<commit_message>
color fill for other types
</commit_message>
<xml_diff>
--- a/test/output/data_schema_properties_2016.xlsx
+++ b/test/output/data_schema_properties_2016.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
   <si>
     <t>column</t>
   </si>
@@ -47,7 +47,7 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>[14629840, 12521812, 10760672, 76914970, 11709999]</t>
+    <t>[11475661, 12226447, 14693504, 14389686, 11431625]</t>
   </si>
   <si>
     <t>airconditioningtypeid</t>
@@ -59,265 +59,271 @@
     <t>architecturalstyletypeid</t>
   </si>
   <si>
+    <t>[7.0, 7.0, 7.0, 7.0, 8.0]</t>
+  </si>
+  <si>
+    <t>basementsqft</t>
+  </si>
+  <si>
+    <t>[308.0, 651.0, 220.0, 1179.0, 228.0]</t>
+  </si>
+  <si>
+    <t>bathroomcnt</t>
+  </si>
+  <si>
+    <t>[1.0, 1.0, 3.0, 2.5, 2.0]</t>
+  </si>
+  <si>
+    <t>bedroomcnt</t>
+  </si>
+  <si>
+    <t>[4.0, 2.0, 4.0, 4.0, 4.0]</t>
+  </si>
+  <si>
+    <t>buildingclasstypeid</t>
+  </si>
+  <si>
+    <t>[3.0, 4.0, 4.0, 4.0, 4.0]</t>
+  </si>
+  <si>
+    <t>buildingqualitytypeid</t>
+  </si>
+  <si>
+    <t>[4.0, 7.0, 7.0, 4.0, 7.0]</t>
+  </si>
+  <si>
+    <t>calculatedbathnbr</t>
+  </si>
+  <si>
+    <t>[3.0, 3.0, 1.0, 2.0, 2.0]</t>
+  </si>
+  <si>
+    <t>decktypeid</t>
+  </si>
+  <si>
+    <t>[66.0, 66.0, 66.0, 66.0, 66.0]</t>
+  </si>
+  <si>
+    <t>finishedfloor1squarefeet</t>
+  </si>
+  <si>
+    <t>[1672.0, 989.0, 1551.0, 1401.0, 664.0]</t>
+  </si>
+  <si>
+    <t>calculatedfinishedsquarefeet</t>
+  </si>
+  <si>
+    <t>[1200.0, 1923.0, 1098.0, 2194.0, 1684.0]</t>
+  </si>
+  <si>
+    <t>finishedsquarefeet12</t>
+  </si>
+  <si>
+    <t>[924.0, 1644.0, 4124.0, 1487.0, 2060.0]</t>
+  </si>
+  <si>
+    <t>finishedsquarefeet13</t>
+  </si>
+  <si>
+    <t>[1296.0, 1296.0, 1440.0, 1152.0, 768.0]</t>
+  </si>
+  <si>
+    <t>finishedsquarefeet15</t>
+  </si>
+  <si>
+    <t>[1088.0, 21042.0, 2904.0, 2368.0, 2685.0]</t>
+  </si>
+  <si>
+    <t>finishedsquarefeet50</t>
+  </si>
+  <si>
+    <t>[664.0, 1169.0, 1730.0, 773.0, 924.0]</t>
+  </si>
+  <si>
+    <t>finishedsquarefeet6</t>
+  </si>
+  <si>
+    <t>[1485.0, 1168.0, 861.0, 3843.0, 986.0]</t>
+  </si>
+  <si>
+    <t>fips</t>
+  </si>
+  <si>
+    <t>[6037.0, 6059.0, 6059.0, 6037.0, 6037.0]</t>
+  </si>
+  <si>
+    <t>fireplacecnt</t>
+  </si>
+  <si>
+    <t>[1.0, 1.0, 3.0, 1.0, 1.0]</t>
+  </si>
+  <si>
+    <t>fullbathcnt</t>
+  </si>
+  <si>
+    <t>[2.0, 1.0, 1.0, 2.0, 3.0]</t>
+  </si>
+  <si>
+    <t>garagecarcnt</t>
+  </si>
+  <si>
+    <t>[2.0, 2.0, 2.0, 1.0, 2.0]</t>
+  </si>
+  <si>
+    <t>garagetotalsqft</t>
+  </si>
+  <si>
+    <t>[495.0, 400.0, 504.0, 0.0, 0.0]</t>
+  </si>
+  <si>
+    <t>hashottuborspa</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>[True, True, True, True, True]</t>
+  </si>
+  <si>
+    <t>heatingorsystemtypeid</t>
+  </si>
+  <si>
+    <t>[7.0, 2.0, 2.0, 2.0, 2.0]</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>[33768978.0, 34055117.0, 33805500.0, 34125450.0, 33630976.0]</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>[-118862129.0, -118752767.0, -118131733.0, -118143495.0, -118637816.0]</t>
+  </si>
+  <si>
+    <t>lotsizesquarefeet</t>
+  </si>
+  <si>
+    <t>[4896.0, 6500.0, 4065.0, 7257.0, 4773.0]</t>
+  </si>
+  <si>
+    <t>poolcnt</t>
+  </si>
+  <si>
+    <t>poolsizesum</t>
+  </si>
+  <si>
+    <t>[540.0, 356.0, 442.0, 800.0, 450.0]</t>
+  </si>
+  <si>
+    <t>pooltypeid10</t>
+  </si>
+  <si>
+    <t>pooltypeid2</t>
+  </si>
+  <si>
+    <t>pooltypeid7</t>
+  </si>
+  <si>
+    <t>propertycountylandusecode</t>
+  </si>
+  <si>
+    <t>['122', '34', '010C', '0200', '0200']</t>
+  </si>
+  <si>
+    <t>propertylandusetypeid</t>
+  </si>
+  <si>
+    <t>[261.0, 261.0, 261.0, 261.0, 266.0]</t>
+  </si>
+  <si>
+    <t>propertyzoningdesc</t>
+  </si>
+  <si>
+    <t>['LARS', 'LAR2', 'WCR17500*', 'LAR1', 'LBR1N']</t>
+  </si>
+  <si>
+    <t>rawcensustractandblock</t>
+  </si>
+  <si>
+    <t>[61110077.001038, 60590994.17100699, 60374070.013009, 60375335.032001, 60590993.051006995]</t>
+  </si>
+  <si>
+    <t>regionidcity</t>
+  </si>
+  <si>
+    <t>[10241.0, 37015.0, 12447.0, 21412.0, 5534.0]</t>
+  </si>
+  <si>
+    <t>regionidcounty</t>
+  </si>
+  <si>
+    <t>[3101.0, 3101.0, 3101.0, 3101.0, 1286.0]</t>
+  </si>
+  <si>
+    <t>regionidneighborhood</t>
+  </si>
+  <si>
+    <t>[276157.0, 31817.0, 274857.0, 276119.0, 268551.0]</t>
+  </si>
+  <si>
+    <t>regionidzip</t>
+  </si>
+  <si>
+    <t>[97089.0, 96492.0, 96159.0, 96492.0, 96993.0]</t>
+  </si>
+  <si>
+    <t>roomcnt</t>
+  </si>
+  <si>
+    <t>[0.0, 0.0, 0.0, 0.0, 4.0]</t>
+  </si>
+  <si>
+    <t>storytypeid</t>
+  </si>
+  <si>
     <t>[7.0, 7.0, 7.0, 7.0, 7.0]</t>
   </si>
   <si>
-    <t>basementsqft</t>
-  </si>
-  <si>
-    <t>[406.0, 645.0, 64.0, 600.0, 2029.0]</t>
-  </si>
-  <si>
-    <t>bathroomcnt</t>
-  </si>
-  <si>
-    <t>[2.0, 1.5, 2.0, 2.0, 2.0]</t>
-  </si>
-  <si>
-    <t>bedroomcnt</t>
-  </si>
-  <si>
-    <t>[4.0, 3.0, 2.0, 3.0, 3.0]</t>
-  </si>
-  <si>
-    <t>buildingclasstypeid</t>
-  </si>
-  <si>
-    <t>[4.0, 4.0, 3.0, 4.0, 3.0]</t>
-  </si>
-  <si>
-    <t>buildingqualitytypeid</t>
-  </si>
-  <si>
-    <t>[7.0, 7.0, 4.0, 4.0, 4.0]</t>
-  </si>
-  <si>
-    <t>calculatedbathnbr</t>
-  </si>
-  <si>
-    <t>[3.0, 2.0, 3.0, 1.0, 1.5]</t>
-  </si>
-  <si>
-    <t>decktypeid</t>
-  </si>
-  <si>
-    <t>[66.0, 66.0, 66.0, 66.0, 66.0]</t>
-  </si>
-  <si>
-    <t>finishedfloor1squarefeet</t>
-  </si>
-  <si>
-    <t>[1474.0, 1375.0, 1096.0, 707.0, 1450.0]</t>
-  </si>
-  <si>
-    <t>calculatedfinishedsquarefeet</t>
-  </si>
-  <si>
-    <t>[738.0, 819.0, 700.0, 1156.0, 1708.0]</t>
-  </si>
-  <si>
-    <t>finishedsquarefeet12</t>
-  </si>
-  <si>
-    <t>[1447.0, 1026.0, 1072.0, 1800.0, 1082.0]</t>
-  </si>
-  <si>
-    <t>finishedsquarefeet13</t>
-  </si>
-  <si>
-    <t>[1392.0, 1440.0, 1248.0, 1296.0, 1440.0]</t>
-  </si>
-  <si>
-    <t>finishedsquarefeet15</t>
-  </si>
-  <si>
-    <t>[2208.0, 3264.0, 938.0, 2122.0, 1564.0]</t>
-  </si>
-  <si>
-    <t>finishedsquarefeet50</t>
-  </si>
-  <si>
-    <t>[1040.0, 1070.0, 1453.0, 1756.0, 1473.0]</t>
-  </si>
-  <si>
-    <t>finishedsquarefeet6</t>
-  </si>
-  <si>
-    <t>[1870.0, 1714.0, 3960.0, 2732.0, 5057.0]</t>
-  </si>
-  <si>
-    <t>fips</t>
-  </si>
-  <si>
-    <t>[6037.0, 6037.0, 6037.0, 6037.0, 6037.0]</t>
-  </si>
-  <si>
-    <t>fireplacecnt</t>
-  </si>
-  <si>
-    <t>[1.0, 1.0, 1.0, 1.0, 2.0]</t>
-  </si>
-  <si>
-    <t>fullbathcnt</t>
-  </si>
-  <si>
-    <t>[1.0, 2.0, 1.0, 2.0, 2.0]</t>
-  </si>
-  <si>
-    <t>garagecarcnt</t>
-  </si>
-  <si>
-    <t>[2.0, 2.0, 0.0, 2.0, 2.0]</t>
-  </si>
-  <si>
-    <t>garagetotalsqft</t>
-  </si>
-  <si>
-    <t>[504.0, 666.0, 410.0, 819.0, 484.0]</t>
-  </si>
-  <si>
-    <t>hashottuborspa</t>
-  </si>
-  <si>
-    <t>str</t>
-  </si>
-  <si>
-    <t>[True, True, True, True, True]</t>
-  </si>
-  <si>
-    <t>heatingorsystemtypeid</t>
-  </si>
-  <si>
-    <t>[2.0, 2.0, 7.0, 7.0, 7.0]</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>[34270910.0, 33776477.0, 34089600.0, 34245033.0, 33609900.0]</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>[-118405261.0, -117906703.0, -118482440.0, -118242687.0, -118259205.0]</t>
-  </si>
-  <si>
-    <t>lotsizesquarefeet</t>
-  </si>
-  <si>
-    <t>[18681.0, 23822.0, 7501.0, 3840.0, 5163.0]</t>
-  </si>
-  <si>
-    <t>poolcnt</t>
-  </si>
-  <si>
-    <t>poolsizesum</t>
-  </si>
-  <si>
-    <t>[450.0, 651.0, 358.0, 473.0, 50.0]</t>
-  </si>
-  <si>
-    <t>pooltypeid10</t>
-  </si>
-  <si>
-    <t>pooltypeid2</t>
-  </si>
-  <si>
-    <t>pooltypeid7</t>
-  </si>
-  <si>
-    <t>propertycountylandusecode</t>
-  </si>
-  <si>
-    <t>['0100', '0100', '0100', '122', '0100']</t>
-  </si>
-  <si>
-    <t>propertylandusetypeid</t>
-  </si>
-  <si>
-    <t>[261.0, 261.0, 261.0, 261.0, 261.0]</t>
-  </si>
-  <si>
-    <t>propertyzoningdesc</t>
-  </si>
-  <si>
-    <t>['LAR1', 'LCC2*', 'MNRS', 'LAR1', 'LCR320U*']</t>
-  </si>
-  <si>
-    <t>rawcensustractandblock</t>
-  </si>
-  <si>
-    <t>[60379005.013011001, 60590525.203004003, 60371973.002001002, 60374060.001000002, 60590879.022007994]</t>
-  </si>
-  <si>
-    <t>regionidcity</t>
-  </si>
-  <si>
-    <t>[42150.0, 53636.0, 5534.0, 12447.0, 26531.0]</t>
-  </si>
-  <si>
-    <t>regionidcounty</t>
-  </si>
-  <si>
-    <t>[3101.0, 2061.0, 1286.0, 3101.0, 3101.0]</t>
-  </si>
-  <si>
-    <t>regionidneighborhood</t>
-  </si>
-  <si>
-    <t>[416965.0, 275078.0, 416303.0, 48570.0, 41131.0]</t>
-  </si>
-  <si>
-    <t>regionidzip</t>
-  </si>
-  <si>
-    <t>[97329.0, 96990.0, 96229.0, 96962.0, 96485.0]</t>
-  </si>
-  <si>
-    <t>roomcnt</t>
-  </si>
-  <si>
-    <t>[0.0, 0.0, 6.0, 8.0, 0.0]</t>
-  </si>
-  <si>
-    <t>storytypeid</t>
-  </si>
-  <si>
     <t>threequarterbathnbr</t>
   </si>
   <si>
     <t>typeconstructiontypeid</t>
   </si>
   <si>
-    <t>[6.0, 6.0, 6.0, 6.0, 4.0]</t>
+    <t>[6.0, 6.0, 6.0, 6.0, 6.0]</t>
   </si>
   <si>
     <t>unitcnt</t>
   </si>
   <si>
+    <t>[1.0, 1.0, 1.0, 2.0, 1.0]</t>
+  </si>
+  <si>
     <t>yardbuildingsqft17</t>
   </si>
   <si>
-    <t>[400.0, 450.0, 340.0, 304.0, 176.0]</t>
+    <t>[160.0, 1094.0, 464.0, 288.0, 377.0]</t>
   </si>
   <si>
     <t>yardbuildingsqft26</t>
   </si>
   <si>
-    <t>[113.0, 224.0, 90.0, 100.0, 100.0]</t>
+    <t>[303.0, 225.0, 462.0, 28.0, 70.0]</t>
   </si>
   <si>
     <t>yearbuilt</t>
   </si>
   <si>
-    <t>[1982.0, 1988.0, 1923.0, 1968.0, 1995.0]</t>
+    <t>[1974.0, 1922.0, 1958.0, 1987.0, 1964.0]</t>
   </si>
   <si>
     <t>numberofstories</t>
   </si>
   <si>
-    <t>[1.0, 1.0, 1.0, 2.0, 1.0]</t>
+    <t>[1.0, 2.0, 1.0, 1.0, 2.0]</t>
   </si>
   <si>
     <t>fireplaceflag</t>
@@ -326,13 +332,13 @@
     <t>structuretaxvaluedollarcnt</t>
   </si>
   <si>
-    <t>[94798.0, 416867.0, 140370.0, 89528.0, 177213.0]</t>
+    <t>[338787.0, 249520.0, 98520.0, 162391.0, 88378.0]</t>
   </si>
   <si>
     <t>taxvaluedollarcnt</t>
   </si>
   <si>
-    <t>[445569.0, 532345.0, 235586.0, 374718.0, 553576.0]</t>
+    <t>[75000.0, 1739043.0, 544388.0, 447260.0, 586987.0]</t>
   </si>
   <si>
     <t>assessmentyear</t>
@@ -344,13 +350,13 @@
     <t>landtaxvaluedollarcnt</t>
   </si>
   <si>
-    <t>[15072.0, 145067.0, 85800.0, 110466.0, 46603.0]</t>
+    <t>[69155.0, 1957180.0, 234512.0, 140065.0, 27271.0]</t>
   </si>
   <si>
     <t>taxamount</t>
   </si>
   <si>
-    <t>[3488.4200000000001, 4043.1399999999999, 2342.8200000000002, 1618.1099999999999, 1497.3199999999999]</t>
+    <t>[4389.53, 4956.5, 4774.17, 5547.84, 1304.96]</t>
   </si>
   <si>
     <t>taxdelinquencyflag</t>
@@ -362,13 +368,13 @@
     <t>taxdelinquencyyear</t>
   </si>
   <si>
-    <t>[10.0, 15.0, 13.0, 13.0, 15.0]</t>
+    <t>[9.0, 15.0, 15.0, 15.0, 15.0]</t>
   </si>
   <si>
     <t>censustractandblock</t>
   </si>
   <si>
-    <t>[60375014003004.0, 60374033163003.0, 60374027031003.0, 60374086302010.0, 60371371031000.0]</t>
+    <t>[60375545221006.0, 60375017002008.0, 60371203001005.0, 60374812013007.0, 61110054011022.0]</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
     <cellStyle builtinId="45" hidden="0" name="Accent5" xfId="1"/>
     <cellStyle builtinId="28" hidden="0" name="Neutral" xfId="2"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="009C0006"/>
@@ -472,6 +478,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="00C6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="0008306B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="009ECAE1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="00A63603"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00FDD0A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="003F007D"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00DADAEB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -778,13 +814,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="42"/>
-    <col customWidth="1" max="2" min="2" width="30"/>
+    <col customWidth="1" max="2" min="2" width="15"/>
     <col customWidth="1" max="3" min="3" width="100"/>
-    <col customWidth="1" max="4" min="4" width="30"/>
-    <col customWidth="1" max="5" min="5" width="30"/>
-    <col customWidth="1" max="6" min="6" width="30"/>
-    <col customWidth="1" max="7" min="7" width="30"/>
-    <col customWidth="1" max="8" min="8" width="30"/>
+    <col customWidth="1" max="4" min="4" width="21"/>
+    <col customWidth="1" max="5" min="5" width="18"/>
+    <col customWidth="1" max="6" min="6" width="24"/>
+    <col customWidth="1" max="7" min="7" width="25.5"/>
+    <col customWidth="1" max="8" min="8" width="25.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="20" r="0" spans="1:8"/>
@@ -1888,7 +1924,7 @@
         <v>9</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="D43" s="4" t="n">
         <v>1</v>
@@ -1908,7 +1944,7 @@
     </row>
     <row customHeight="1" ht="20" r="44" spans="1:8">
       <c r="A44" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>9</v>
@@ -1934,13 +1970,13 @@
     </row>
     <row customHeight="1" ht="20" r="45" spans="1:8">
       <c r="A45" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D45" s="4" t="n">
         <v>5</v>
@@ -1960,13 +1996,13 @@
     </row>
     <row customHeight="1" ht="20" r="46" spans="1:8">
       <c r="A46" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="D46" s="4" t="n">
         <v>146</v>
@@ -1986,13 +2022,13 @@
     </row>
     <row customHeight="1" ht="20" r="47" spans="1:8">
       <c r="A47" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D47" s="4" t="n">
         <v>1636</v>
@@ -2012,13 +2048,13 @@
     </row>
     <row customHeight="1" ht="20" r="48" spans="1:8">
       <c r="A48" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D48" s="4" t="n">
         <v>594</v>
@@ -2038,13 +2074,13 @@
     </row>
     <row customHeight="1" ht="20" r="49" spans="1:8">
       <c r="A49" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D49" s="4" t="n">
         <v>168</v>
@@ -2064,13 +2100,13 @@
     </row>
     <row customHeight="1" ht="20" r="50" spans="1:8">
       <c r="A50" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D50" s="4" t="n">
         <v>12</v>
@@ -2090,7 +2126,7 @@
     </row>
     <row customHeight="1" ht="20" r="51" spans="1:8">
       <c r="A51" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>54</v>
@@ -2116,13 +2152,13 @@
     </row>
     <row customHeight="1" ht="20" r="52" spans="1:8">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D52" s="4" t="n">
         <v>426150</v>
@@ -2142,13 +2178,13 @@
     </row>
     <row customHeight="1" ht="20" r="53" spans="1:8">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D53" s="4" t="n">
         <v>638920</v>
@@ -2168,13 +2204,13 @@
     </row>
     <row customHeight="1" ht="20" r="54" spans="1:8">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D54" s="4" t="n">
         <v>14</v>
@@ -2194,13 +2230,13 @@
     </row>
     <row customHeight="1" ht="20" r="55" spans="1:8">
       <c r="A55" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D55" s="4" t="n">
         <v>531408</v>
@@ -2220,13 +2256,13 @@
     </row>
     <row customHeight="1" ht="20" r="56" spans="1:8">
       <c r="A56" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D56" s="4" t="n">
         <v>1045757</v>
@@ -2246,13 +2282,13 @@
     </row>
     <row customHeight="1" ht="20" r="57" spans="1:8">
       <c r="A57" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D57" s="4" t="n">
         <v>1</v>
@@ -2272,13 +2308,13 @@
     </row>
     <row customHeight="1" ht="20" r="58" spans="1:8">
       <c r="A58" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D58" s="4" t="n">
         <v>32</v>
@@ -2298,13 +2334,13 @@
     </row>
     <row customHeight="1" ht="20" r="59" spans="1:8">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D59" s="4" t="n">
         <v>96771</v>
@@ -2330,12 +2366,21 @@
     <cfRule dxfId="1" priority="2" stopIfTrue="1" type="expression">
       <formula>B2="key"</formula>
     </cfRule>
+    <cfRule dxfId="2" priority="3" stopIfTrue="1" type="expression">
+      <formula>B2="numeric"</formula>
+    </cfRule>
+    <cfRule dxfId="3" priority="4" stopIfTrue="1" type="expression">
+      <formula>B2="str"</formula>
+    </cfRule>
+    <cfRule dxfId="4" priority="5" stopIfTrue="1" type="expression">
+      <formula>B2="date"</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D59">
-    <cfRule dxfId="0" priority="3" stopIfTrue="1" type="expression">
+    <cfRule dxfId="0" priority="6" stopIfTrue="1" type="expression">
       <formula>D2=0</formula>
     </cfRule>
-    <cfRule dxfId="0" priority="4" stopIfTrue="1" type="expression">
+    <cfRule dxfId="0" priority="7" stopIfTrue="1" type="expression">
       <formula>D2=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>